<commit_message>
CA MU addr seq length fix
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateAutoCA.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateAutoCA.xlsx
@@ -3151,9 +3151,12 @@
   <mergeCells>
     <mergeCell ref="A2002:Q2002"/>
   </mergeCells>
-  <dataValidations count="16">
+  <dataValidations count="17">
     <dataValidation type="textLength" operator="equal" sqref="A2:A2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Value should be exactly 6 characters long." showInputMessage="true" promptTitle="Note:" prompt="Value should be exactly 6 characters long.">
       <formula1>6</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" sqref="B2:B2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Value should be exactly 5 characters long." showInputMessage="true" promptTitle="Note:" prompt="Value should be exactly 5 characters long.">
+      <formula1>5</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" sqref="C2:C2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Maximum length of the value is 30 characters." showInputMessage="true" promptTitle="Note:" prompt="Maximum length of the value is 30 characters.">
       <formula1>30</formula1>
@@ -3297,9 +3300,12 @@
   <mergeCells>
     <mergeCell ref="A2002:Q2002"/>
   </mergeCells>
-  <dataValidations count="16">
+  <dataValidations count="17">
     <dataValidation type="textLength" operator="equal" sqref="A2:A2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Value should be exactly 6 characters long." showInputMessage="true" promptTitle="Note:" prompt="Value should be exactly 6 characters long.">
       <formula1>6</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" sqref="B2:B2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Value should be exactly 5 characters long." showInputMessage="true" promptTitle="Note:" prompt="Value should be exactly 5 characters long.">
+      <formula1>5</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" sqref="C2:C2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Maximum length of the value is 30 characters." showInputMessage="true" promptTitle="Note:" prompt="Maximum length of the value is 30 characters.">
       <formula1>30</formula1>

</xml_diff>